<commit_message>
hopefully final data I swear
</commit_message>
<xml_diff>
--- a/All_data.xlsx
+++ b/All_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thertzell/fluffy-journey-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125CB843-7275-9E42-94C6-889B2790D692}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD965A3-3222-7742-9C31-89012D736E8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22640" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -285,7 +285,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -293,12 +293,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -367,20 +361,14 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1552,10 +1540,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U67"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="Q46" sqref="M17:Q46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1568,2207 +1556,2150 @@
     <col min="8" max="8" width="6" style="1" customWidth="1"/>
     <col min="9" max="9" width="3.83203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="4.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="4.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="5.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.6640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="8.83203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="6" style="1" customWidth="1"/>
-    <col min="19" max="19" width="3.83203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="6.5" style="1" customWidth="1"/>
-    <col min="21" max="21" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.33203125" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.33203125" style="1"/>
+    <col min="11" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>0.41200000000000003</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>0.72199999999999998</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>0.55299999999999994</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>4</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>3</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>16</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>0.57799999999999996</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>0.623</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>0.56299999999999994</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>13</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>12</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <v>61</v>
       </c>
-      <c r="J3" s="3">
-        <v>11</v>
-      </c>
-      <c r="L3" s="4"/>
-    </row>
-    <row r="4" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
+      <c r="J3" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>0.33299999999999996</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.49299999999999999</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>0.49200000000000005</v>
       </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3">
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
         <v>58</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
         <v>0.69200000000000006</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>0.49399999999999999</v>
       </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3">
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
         <v>7</v>
       </c>
-      <c r="J5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="6" t="s">
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
         <v>0.125</v>
       </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3">
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
         <v>1</v>
       </c>
-      <c r="J6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="6" t="s">
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
         <v>0.61699999999999999</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>0.51400000000000001</v>
       </c>
-      <c r="G7" s="3">
-        <v>11</v>
-      </c>
-      <c r="H7" s="3">
+      <c r="G7" s="2">
+        <v>11</v>
+      </c>
+      <c r="H7" s="2">
         <v>9</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>67</v>
       </c>
-      <c r="J7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="6" t="s">
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>0.5</v>
       </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3">
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
         <v>0.63500000000000001</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>1</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>1</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>3</v>
       </c>
-      <c r="J8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
         <v>0.55500000000000005</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>0.46700000000000003</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>23</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>18</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>68</v>
       </c>
-      <c r="J9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="6" t="s">
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
         <v>0.37</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>0.46600000000000003</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>6</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>6</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <v>31</v>
       </c>
-      <c r="J10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>0.46600000000000003</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>0.60399999999999998</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>0.51300000000000001</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>9</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>8</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <v>70</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>0.34600000000000003</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>0.61899999999999999</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>0.52</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>7</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>7</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <v>65</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3">
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
         <v>1</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="G13" s="3">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3">
-        <v>0</v>
-      </c>
-      <c r="I13" s="3">
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
         <v>2</v>
       </c>
-      <c r="J13" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="6" t="s">
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="B14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3">
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
         <v>0.125</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="2">
         <v>1</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="2">
         <v>1</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="2">
         <v>1</v>
       </c>
-      <c r="J14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="6" t="s">
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
         <v>0.53600000000000003</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>0.51800000000000002</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="2">
         <v>17</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="2">
         <v>17</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="2">
         <v>68</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="7" t="s">
+      <c r="B16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>0.41700000000000004</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>0.61199999999999999</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <v>0.48</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="2">
         <v>4</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="2">
         <v>4</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="2">
         <v>58</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="B17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="3">
-        <v>0</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0</v>
-      </c>
-      <c r="F17" s="3">
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
         <v>0.35700000000000004</v>
       </c>
-      <c r="G17" s="3">
-        <v>0</v>
-      </c>
-      <c r="H17" s="3">
-        <v>0</v>
-      </c>
-      <c r="I17" s="3">
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
         <v>1</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="B18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="3">
-        <v>0</v>
-      </c>
-      <c r="E18" s="3">
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
         <v>0.46399999999999997</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
         <v>0.505</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="2">
         <v>1</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="2">
         <v>1</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="2">
         <v>10</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="7" t="s">
+      <c r="B19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="3">
-        <v>0</v>
-      </c>
-      <c r="E19" s="3">
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
         <v>0.64300000000000002</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <v>0.47299999999999998</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="2">
         <v>2</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="2">
         <v>2</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="2">
         <v>6</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>0.502</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>0.50900000000000001</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>0.51300000000000001</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <v>9</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="2">
         <v>7</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="2">
         <v>61</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="B21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="3">
-        <v>0</v>
-      </c>
-      <c r="E21" s="3">
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
         <v>0.52700000000000002</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <v>0.56200000000000006</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="2">
         <v>15</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="2">
         <v>14</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="2">
         <v>61</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="B22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>0.25</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>0.6</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>0.54400000000000004</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="2">
         <v>5</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="2">
         <v>4</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="2">
         <v>25</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="7" t="s">
+      <c r="B23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>0.48799999999999999</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>0.57200000000000006</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>0.45799999999999996</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="2">
         <v>13</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="2">
         <v>12</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="2">
         <v>69</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="7" t="s">
+      <c r="B24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="3">
-        <v>0</v>
-      </c>
-      <c r="E24" s="3">
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
         <v>0.60599999999999998</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <v>0.46799999999999997</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="2">
         <v>9</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="2">
         <v>7</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="2">
         <v>19</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="7" t="s">
+      <c r="B25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>0.45799999999999996</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <v>0.58299999999999996</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="2">
         <v>0.47</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="2">
         <v>1</v>
       </c>
-      <c r="H25" s="3">
-        <v>0</v>
-      </c>
-      <c r="I25" s="3">
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2">
         <v>40</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="7" t="s">
+      <c r="B26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>0.43099999999999999</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>0.61499999999999999</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="2">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="2">
         <v>33</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="2">
         <v>29</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="2">
         <v>70</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="7" t="s">
+      <c r="B27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="3">
-        <v>0</v>
-      </c>
-      <c r="E27" s="3">
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
         <v>0.45899999999999996</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="2">
         <v>0.51300000000000001</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="2">
         <v>19</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="2">
         <v>18</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27" s="2">
         <v>67</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="7" t="s">
+      <c r="B28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="3">
-        <v>0</v>
-      </c>
-      <c r="E28" s="3">
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
         <v>0.48499999999999999</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="2">
         <v>0.49700000000000005</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28" s="2">
         <v>4</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="2">
         <v>3</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28" s="2">
         <v>24</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="B29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>0.14300000000000002</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <v>0.55700000000000005</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="2">
         <v>0.42399999999999999</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="2">
         <v>7</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="2">
         <v>6</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29" s="2">
         <v>48</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="7" t="s">
+      <c r="B30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="2">
         <v>0.38900000000000001</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <v>0.55100000000000005</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="2">
         <v>0.55299999999999994</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="2">
         <v>20</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="2">
         <v>20</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="2">
         <v>70</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30" s="2">
         <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="7" t="s">
+      <c r="B31" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="2">
         <v>0.4</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <v>0.59599999999999997</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="2">
         <v>0.51100000000000001</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="2">
         <v>5</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="2">
         <v>3</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31" s="2">
         <v>27</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="7" t="s">
+      <c r="B32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="3">
-        <v>0</v>
-      </c>
-      <c r="E32" s="3">
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
         <v>0.5</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="2">
         <v>0.48899999999999999</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G32" s="2">
         <v>4</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="2">
         <v>2</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32" s="2">
         <v>7</v>
       </c>
-      <c r="J32" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="6" t="s">
+      <c r="J32" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="7" t="s">
+      <c r="B33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="2">
         <v>1</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="2">
         <v>0.25</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="2">
         <v>0.57799999999999996</v>
       </c>
-      <c r="G33" s="3">
-        <v>0</v>
-      </c>
-      <c r="H33" s="3">
-        <v>0</v>
-      </c>
-      <c r="I33" s="3">
+      <c r="G33" s="2">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0</v>
+      </c>
+      <c r="I33" s="2">
         <v>4</v>
       </c>
-      <c r="J33" s="3">
-        <v>0</v>
-      </c>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
-    </row>
-    <row r="34" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="6" t="s">
+      <c r="J33" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="7" t="s">
+      <c r="B34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="2">
         <v>0.6</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="2">
         <v>0.75</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="2">
         <v>0.51400000000000001</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34" s="2">
         <v>1</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="2">
         <v>1</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34" s="2">
         <v>2</v>
       </c>
-      <c r="J34" s="3">
-        <v>0</v>
-      </c>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="2"/>
-      <c r="U34" s="2"/>
-    </row>
-    <row r="35" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="6" t="s">
+      <c r="J34" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="7" t="s">
+      <c r="B35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="3">
-        <v>0</v>
-      </c>
-      <c r="E35" s="3">
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
         <v>0.222</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="2">
         <v>0.36799999999999999</v>
       </c>
-      <c r="G35" s="3">
-        <v>0</v>
-      </c>
-      <c r="H35" s="3">
-        <v>0</v>
-      </c>
-      <c r="I35" s="3">
+      <c r="G35" s="2">
+        <v>0</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0</v>
+      </c>
+      <c r="I35" s="2">
         <v>5</v>
       </c>
-      <c r="J35" s="3">
-        <v>0</v>
-      </c>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-      <c r="Q35" s="2"/>
-      <c r="R35" s="2"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="2"/>
-      <c r="U35" s="2"/>
-    </row>
-    <row r="36" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="6" t="s">
+      <c r="J35" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="7" t="s">
+      <c r="B36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="2">
         <v>0.46200000000000002</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="2">
         <v>0.56100000000000005</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="2">
         <v>0.45200000000000001</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36" s="2">
         <v>19</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H36" s="2">
         <v>16</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I36" s="2">
         <v>67</v>
       </c>
-      <c r="J36" s="3">
-        <v>0</v>
-      </c>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="2"/>
-      <c r="R36" s="2"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="2"/>
-      <c r="U36" s="2"/>
-    </row>
-    <row r="37" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="7" t="s">
+      <c r="J36" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="3">
-        <v>0</v>
-      </c>
-      <c r="E37" s="3">
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2">
         <v>0.4</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="2">
         <v>0.4</v>
       </c>
-      <c r="G37" s="3">
-        <v>0</v>
-      </c>
-      <c r="H37" s="3">
-        <v>0</v>
-      </c>
-      <c r="I37" s="3">
+      <c r="G37" s="2">
+        <v>0</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0</v>
+      </c>
+      <c r="I37" s="2">
         <v>1</v>
       </c>
-      <c r="J37" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="7" t="s">
+      <c r="J37" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="3">
-        <v>0</v>
-      </c>
-      <c r="E38" s="3">
+      <c r="D38" s="2">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2">
         <v>0.46700000000000003</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38" s="2">
         <v>0.47899999999999998</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G38" s="2">
         <v>3</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="2">
         <v>3</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38" s="2">
         <v>41</v>
       </c>
-      <c r="J38" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="7" t="s">
+      <c r="J38" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="2">
         <v>0.28600000000000003</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="2">
         <v>0.65900000000000003</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39" s="2">
         <v>0.48200000000000004</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G39" s="2">
         <v>13</v>
       </c>
-      <c r="H39" s="3">
-        <v>11</v>
-      </c>
-      <c r="I39" s="3">
+      <c r="H39" s="2">
+        <v>11</v>
+      </c>
+      <c r="I39" s="2">
         <v>40</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J39" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="7" t="s">
+    <row r="40" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="3">
-        <v>0</v>
-      </c>
-      <c r="E40" s="3">
+      <c r="D40" s="2">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2">
         <v>0.33299999999999996</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40" s="2">
         <v>0.496</v>
       </c>
-      <c r="G40" s="3">
-        <v>0</v>
-      </c>
-      <c r="H40" s="3">
-        <v>0</v>
-      </c>
-      <c r="I40" s="3">
+      <c r="G40" s="2">
+        <v>0</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0</v>
+      </c>
+      <c r="I40" s="2">
         <v>6</v>
       </c>
-      <c r="J40" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="7" t="s">
+      <c r="J40" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="2">
         <v>0.43099999999999999</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="2">
         <v>0.63</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41" s="2">
         <v>0.47100000000000003</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G41" s="2">
         <v>10</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41" s="2">
         <v>9</v>
       </c>
-      <c r="I41" s="3">
+      <c r="I41" s="2">
         <v>69</v>
       </c>
-      <c r="J41" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="7" t="s">
+      <c r="J41" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="2">
         <v>0.33799999999999997</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="2">
         <v>0.623</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="2">
         <v>0.48399999999999999</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G42" s="2">
         <v>12</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42" s="2">
         <v>12</v>
       </c>
-      <c r="I42" s="3">
+      <c r="I42" s="2">
         <v>64</v>
       </c>
-      <c r="J42" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="7" t="s">
+      <c r="J42" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D43" s="3">
-        <v>0</v>
-      </c>
-      <c r="E43" s="3">
+      <c r="D43" s="2">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2">
         <v>0.442</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43" s="2">
         <v>0.47499999999999998</v>
       </c>
-      <c r="G43" s="3">
+      <c r="G43" s="2">
         <v>5</v>
       </c>
-      <c r="H43" s="3">
+      <c r="H43" s="2">
         <v>5</v>
       </c>
-      <c r="I43" s="3">
+      <c r="I43" s="2">
         <v>29</v>
       </c>
-      <c r="J43" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="7" t="s">
+      <c r="J43" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="2">
         <v>0.35</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="2">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44" s="2">
         <v>0.501</v>
       </c>
-      <c r="G44" s="3">
+      <c r="G44" s="2">
         <v>6</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H44" s="2">
         <v>5</v>
       </c>
-      <c r="I44" s="3">
+      <c r="I44" s="2">
         <v>70</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="7" t="s">
+    <row r="45" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="3">
-        <v>0</v>
-      </c>
-      <c r="E45" s="3">
+      <c r="D45" s="2">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2">
         <v>0.63200000000000001</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45" s="2">
         <v>0.43</v>
       </c>
-      <c r="G45" s="3">
+      <c r="G45" s="2">
         <v>9</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H45" s="2">
         <v>4</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I45" s="2">
         <v>21</v>
       </c>
-      <c r="J45" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="7" t="s">
+      <c r="J45" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="3">
-        <v>0</v>
-      </c>
-      <c r="E46" s="3">
+      <c r="D46" s="2">
+        <v>0</v>
+      </c>
+      <c r="E46" s="2">
         <v>0.41700000000000004</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F46" s="2">
         <v>0.504</v>
       </c>
-      <c r="G46" s="3">
-        <v>11</v>
-      </c>
-      <c r="H46" s="3">
+      <c r="G46" s="2">
+        <v>11</v>
+      </c>
+      <c r="H46" s="2">
         <v>10</v>
       </c>
-      <c r="I46" s="3">
+      <c r="I46" s="2">
         <v>59</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J46" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="7" t="s">
+    <row r="47" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D47" s="3">
-        <v>0</v>
-      </c>
-      <c r="E47" s="3">
+      <c r="D47" s="2">
+        <v>0</v>
+      </c>
+      <c r="E47" s="2">
         <v>0.8</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F47" s="2">
         <v>0.43799999999999994</v>
       </c>
-      <c r="G47" s="3">
-        <v>0</v>
-      </c>
-      <c r="H47" s="3">
-        <v>0</v>
-      </c>
-      <c r="I47" s="3">
+      <c r="G47" s="2">
+        <v>0</v>
+      </c>
+      <c r="H47" s="2">
+        <v>0</v>
+      </c>
+      <c r="I47" s="2">
         <v>1</v>
       </c>
-      <c r="J47" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="7" t="s">
+      <c r="J47" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="2">
         <v>0.25</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="2">
         <v>0.57399999999999995</v>
       </c>
-      <c r="F48" s="3">
+      <c r="F48" s="2">
         <v>0.46500000000000002</v>
       </c>
-      <c r="G48" s="3">
+      <c r="G48" s="2">
         <v>3</v>
       </c>
-      <c r="H48" s="3">
+      <c r="H48" s="2">
         <v>3</v>
       </c>
-      <c r="I48" s="3">
+      <c r="I48" s="2">
         <v>36</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="2">
         <v>0.52300000000000002</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="2">
         <v>0.64300000000000002</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F49" s="2">
         <v>0.47899999999999998</v>
       </c>
-      <c r="G49" s="3">
+      <c r="G49" s="2">
         <v>4</v>
       </c>
-      <c r="H49" s="3">
+      <c r="H49" s="2">
         <v>4</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I49" s="2">
         <v>70</v>
       </c>
-      <c r="J49" s="3">
+      <c r="J49" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="2">
         <v>0.25</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="2">
         <v>0.59299999999999997</v>
       </c>
-      <c r="F50" s="3">
+      <c r="F50" s="2">
         <v>0.49099999999999999</v>
       </c>
-      <c r="G50" s="3">
+      <c r="G50" s="2">
         <v>16</v>
       </c>
-      <c r="H50" s="3">
+      <c r="H50" s="2">
         <v>15</v>
       </c>
-      <c r="I50" s="3">
+      <c r="I50" s="2">
         <v>70</v>
       </c>
-      <c r="J50" s="3">
+      <c r="J50" s="2">
         <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D51" s="3">
-        <v>0</v>
-      </c>
-      <c r="E51" s="3">
+      <c r="D51" s="2">
+        <v>0</v>
+      </c>
+      <c r="E51" s="2">
         <v>0.434</v>
       </c>
-      <c r="F51" s="3">
+      <c r="F51" s="2">
         <v>0.49099999999999999</v>
       </c>
-      <c r="G51" s="3">
+      <c r="G51" s="2">
         <v>9</v>
       </c>
-      <c r="H51" s="3">
+      <c r="H51" s="2">
         <v>9</v>
       </c>
-      <c r="I51" s="3">
+      <c r="I51" s="2">
         <v>61</v>
       </c>
-      <c r="J51" s="3">
+      <c r="J51" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C52" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="3">
-        <v>0</v>
-      </c>
-      <c r="E52" s="3">
+      <c r="D52" s="2">
+        <v>0</v>
+      </c>
+      <c r="E52" s="2">
         <v>0.40200000000000002</v>
       </c>
-      <c r="F52" s="3">
+      <c r="F52" s="2">
         <v>0.52500000000000002</v>
       </c>
-      <c r="G52" s="3">
+      <c r="G52" s="2">
         <v>17</v>
       </c>
-      <c r="H52" s="3">
+      <c r="H52" s="2">
         <v>16</v>
       </c>
-      <c r="I52" s="3">
+      <c r="I52" s="2">
         <v>42</v>
       </c>
-      <c r="J52" s="3">
+      <c r="J52" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="2">
         <v>0.316</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E53" s="2">
         <v>0.58099999999999996</v>
       </c>
-      <c r="F53" s="3">
+      <c r="F53" s="2">
         <v>0.501</v>
       </c>
-      <c r="G53" s="3">
+      <c r="G53" s="2">
         <v>8</v>
       </c>
-      <c r="H53" s="3">
+      <c r="H53" s="2">
         <v>8</v>
       </c>
-      <c r="I53" s="3">
+      <c r="I53" s="2">
         <v>68</v>
       </c>
-      <c r="J53" s="3">
+      <c r="J53" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C54" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D54" s="3">
-        <v>0</v>
-      </c>
-      <c r="E54" s="3">
+      <c r="D54" s="2">
+        <v>0</v>
+      </c>
+      <c r="E54" s="2">
         <v>0.47299999999999998</v>
       </c>
-      <c r="F54" s="3">
+      <c r="F54" s="2">
         <v>0.49200000000000005</v>
       </c>
-      <c r="G54" s="3">
+      <c r="G54" s="2">
         <v>10</v>
       </c>
-      <c r="H54" s="3">
+      <c r="H54" s="2">
         <v>10</v>
       </c>
-      <c r="I54" s="3">
+      <c r="I54" s="2">
         <v>65</v>
       </c>
-      <c r="J54" s="3">
+      <c r="J54" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D55" s="3">
-        <v>0</v>
-      </c>
-      <c r="E55" s="3">
+      <c r="D55" s="2">
+        <v>0</v>
+      </c>
+      <c r="E55" s="2">
         <v>0.496</v>
       </c>
-      <c r="F55" s="3">
+      <c r="F55" s="2">
         <v>0.496</v>
       </c>
-      <c r="G55" s="3">
+      <c r="G55" s="2">
         <v>12</v>
       </c>
-      <c r="H55" s="3">
-        <v>11</v>
-      </c>
-      <c r="I55" s="3">
+      <c r="H55" s="2">
+        <v>11</v>
+      </c>
+      <c r="I55" s="2">
         <v>58</v>
       </c>
-      <c r="J55" s="3">
+      <c r="J55" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C56" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D56" s="2">
         <v>0.26300000000000001</v>
       </c>
-      <c r="E56" s="3">
+      <c r="E56" s="2">
         <v>0.623</v>
       </c>
-      <c r="F56" s="3">
+      <c r="F56" s="2">
         <v>0.49399999999999999</v>
       </c>
-      <c r="G56" s="3">
+      <c r="G56" s="2">
         <v>5</v>
       </c>
-      <c r="H56" s="3">
+      <c r="H56" s="2">
         <v>5</v>
       </c>
-      <c r="I56" s="3">
+      <c r="I56" s="2">
         <v>65</v>
       </c>
-      <c r="J56" s="3">
+      <c r="J56" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C57" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D57" s="3">
-        <v>0</v>
-      </c>
-      <c r="E57" s="3">
+      <c r="D57" s="2">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2">
         <v>0.5</v>
       </c>
-      <c r="F57" s="3">
+      <c r="F57" s="2">
         <v>0.66700000000000004</v>
       </c>
-      <c r="G57" s="3">
-        <v>0</v>
-      </c>
-      <c r="H57" s="3">
-        <v>0</v>
-      </c>
-      <c r="I57" s="3">
+      <c r="G57" s="2">
+        <v>0</v>
+      </c>
+      <c r="H57" s="2">
+        <v>0</v>
+      </c>
+      <c r="I57" s="2">
         <v>1</v>
       </c>
-      <c r="J57" s="3">
+      <c r="J57" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C58" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D58" s="3">
+      <c r="D58" s="2">
         <v>0.75</v>
       </c>
-      <c r="E58" s="3">
+      <c r="E58" s="2">
         <v>0.73699999999999999</v>
       </c>
-      <c r="F58" s="3">
+      <c r="F58" s="2">
         <v>0.51</v>
       </c>
-      <c r="G58" s="3">
-        <v>0</v>
-      </c>
-      <c r="H58" s="3">
-        <v>0</v>
-      </c>
-      <c r="I58" s="3">
+      <c r="G58" s="2">
+        <v>0</v>
+      </c>
+      <c r="H58" s="2">
+        <v>0</v>
+      </c>
+      <c r="I58" s="2">
         <v>9</v>
       </c>
-      <c r="J58" s="3">
+      <c r="J58" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D59" s="2">
         <v>0.39700000000000002</v>
       </c>
-      <c r="E59" s="3">
+      <c r="E59" s="2">
         <v>0.65400000000000003</v>
       </c>
-      <c r="F59" s="3">
+      <c r="F59" s="2">
         <v>0.51100000000000001</v>
       </c>
-      <c r="G59" s="3">
+      <c r="G59" s="2">
         <v>8</v>
       </c>
-      <c r="H59" s="3">
+      <c r="H59" s="2">
         <v>8</v>
       </c>
-      <c r="I59" s="3">
+      <c r="I59" s="2">
         <v>58</v>
       </c>
-      <c r="J59" s="3">
+      <c r="J59" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D60" s="3">
-        <v>0</v>
-      </c>
-      <c r="E60" s="3">
+      <c r="D60" s="2">
+        <v>0</v>
+      </c>
+      <c r="E60" s="2">
         <v>0.51300000000000001</v>
       </c>
-      <c r="F60" s="3">
+      <c r="F60" s="2">
         <v>0.44400000000000001</v>
       </c>
-      <c r="G60" s="3">
+      <c r="G60" s="2">
         <v>4</v>
       </c>
-      <c r="H60" s="3">
+      <c r="H60" s="2">
         <v>4</v>
       </c>
-      <c r="I60" s="3">
+      <c r="I60" s="2">
         <v>32</v>
       </c>
-      <c r="J60" s="3">
+      <c r="J60" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D61" s="3">
-        <v>0</v>
-      </c>
-      <c r="E61" s="3">
+      <c r="D61" s="2">
+        <v>0</v>
+      </c>
+      <c r="E61" s="2">
         <v>0.16699999999999998</v>
       </c>
-      <c r="F61" s="3">
+      <c r="F61" s="2">
         <v>0.38900000000000001</v>
       </c>
-      <c r="G61" s="3">
+      <c r="G61" s="2">
         <v>2</v>
       </c>
-      <c r="H61" s="3">
+      <c r="H61" s="2">
         <v>1</v>
       </c>
-      <c r="I61" s="3">
+      <c r="I61" s="2">
         <v>6</v>
       </c>
-      <c r="J61" s="3">
+      <c r="J61" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C62" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D62" s="3">
+      <c r="D62" s="2">
         <v>0.45200000000000001</v>
       </c>
-      <c r="E62" s="3">
+      <c r="E62" s="2">
         <v>0.66700000000000004</v>
       </c>
-      <c r="F62" s="3">
+      <c r="F62" s="2">
         <v>0.52200000000000002</v>
       </c>
-      <c r="G62" s="3">
+      <c r="G62" s="2">
         <v>15</v>
       </c>
-      <c r="H62" s="3">
+      <c r="H62" s="2">
         <v>14</v>
       </c>
-      <c r="I62" s="3">
+      <c r="I62" s="2">
         <v>26</v>
       </c>
-      <c r="J62" s="3">
+      <c r="J62" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C63" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D63" s="3">
-        <v>0</v>
-      </c>
-      <c r="E63" s="3">
+      <c r="D63" s="2">
+        <v>0</v>
+      </c>
+      <c r="E63" s="2">
         <v>0.83299999999999996</v>
       </c>
-      <c r="F63" s="3">
+      <c r="F63" s="2">
         <v>0.48200000000000004</v>
       </c>
-      <c r="G63" s="3">
-        <v>0</v>
-      </c>
-      <c r="H63" s="3">
-        <v>0</v>
-      </c>
-      <c r="I63" s="3">
+      <c r="G63" s="2">
+        <v>0</v>
+      </c>
+      <c r="H63" s="2">
+        <v>0</v>
+      </c>
+      <c r="I63" s="2">
         <v>9</v>
       </c>
-      <c r="J63" s="3">
+      <c r="J63" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C64" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D64" s="2">
         <v>0.46299999999999997</v>
       </c>
-      <c r="E64" s="3">
+      <c r="E64" s="2">
         <v>0.56600000000000006</v>
       </c>
-      <c r="F64" s="3">
+      <c r="F64" s="2">
         <v>0.46200000000000002</v>
       </c>
-      <c r="G64" s="3">
+      <c r="G64" s="2">
         <v>13</v>
       </c>
-      <c r="H64" s="3">
+      <c r="H64" s="2">
         <v>12</v>
       </c>
-      <c r="I64" s="3">
+      <c r="I64" s="2">
         <v>50</v>
       </c>
-      <c r="J64" s="3">
+      <c r="J64" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="7" t="s">
+      <c r="A65" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C65" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D65" s="3">
+      <c r="D65" s="2">
         <v>0.47700000000000004</v>
       </c>
-      <c r="E65" s="3">
+      <c r="E65" s="2">
         <v>0.66</v>
       </c>
-      <c r="F65" s="3">
+      <c r="F65" s="2">
         <v>0.49700000000000005</v>
       </c>
-      <c r="G65" s="3">
+      <c r="G65" s="2">
         <v>8</v>
       </c>
-      <c r="H65" s="3">
+      <c r="H65" s="2">
         <v>8</v>
       </c>
-      <c r="I65" s="3">
+      <c r="I65" s="2">
         <v>58</v>
       </c>
-      <c r="J65" s="3">
+      <c r="J65" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="7" t="s">
+      <c r="A66" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B66" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C66" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D66" s="3">
+      <c r="D66" s="2">
         <v>0.57299999999999995</v>
       </c>
-      <c r="E66" s="3">
+      <c r="E66" s="2">
         <v>0.60399999999999998</v>
       </c>
-      <c r="F66" s="3">
+      <c r="F66" s="2">
         <v>0.505</v>
       </c>
-      <c r="G66" s="3">
+      <c r="G66" s="2">
         <v>23</v>
       </c>
-      <c r="H66" s="3">
+      <c r="H66" s="2">
         <v>22</v>
       </c>
-      <c r="I66" s="3">
+      <c r="I66" s="2">
         <v>70</v>
       </c>
-      <c r="J66" s="3">
+      <c r="J66" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B67" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="C67" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D67" s="3">
-        <v>0</v>
-      </c>
-      <c r="E67" s="3">
+      <c r="D67" s="2">
+        <v>0</v>
+      </c>
+      <c r="E67" s="2">
         <v>0.66700000000000004</v>
       </c>
-      <c r="F67" s="3">
+      <c r="F67" s="2">
         <v>0.43200000000000005</v>
       </c>
-      <c r="G67" s="3">
+      <c r="G67" s="2">
         <v>2</v>
       </c>
-      <c r="H67" s="3">
+      <c r="H67" s="2">
         <v>2</v>
       </c>
-      <c r="I67" s="3">
+      <c r="I67" s="2">
         <v>4</v>
       </c>
-      <c r="J67" s="3">
+      <c r="J67" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>